<commit_message>
data update + axis text rotation
</commit_message>
<xml_diff>
--- a/data/investimentos.xlsx
+++ b/data/investimentos.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="25">
   <si>
     <t xml:space="preserve">nome</t>
   </si>
@@ -104,10 +104,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -201,7 +203,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -258,7 +260,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -279,12 +293,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H65536"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A439" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A552" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E452" activeCellId="0" sqref="E452"/>
+      <selection pane="bottomLeft" activeCell="E565" activeCellId="0" sqref="E565"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7029,7 +7043,7 @@
       <c r="B335" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C335" s="14" t="n">
+      <c r="C335" s="12" t="n">
         <v>43110</v>
       </c>
       <c r="D335" s="13" t="n">
@@ -7043,7 +7057,7 @@
       <c r="B336" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C336" s="14" t="n">
+      <c r="C336" s="12" t="n">
         <v>43110</v>
       </c>
       <c r="D336" s="13" t="n">
@@ -7057,7 +7071,7 @@
       <c r="B337" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C337" s="14" t="n">
+      <c r="C337" s="12" t="n">
         <v>43110</v>
       </c>
       <c r="D337" s="13" t="n">
@@ -7071,7 +7085,7 @@
       <c r="B338" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C338" s="14" t="n">
+      <c r="C338" s="12" t="n">
         <v>43110</v>
       </c>
       <c r="D338" s="13" t="n">
@@ -7085,7 +7099,7 @@
       <c r="B339" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C339" s="14" t="n">
+      <c r="C339" s="12" t="n">
         <v>43110</v>
       </c>
       <c r="D339" s="13" t="n">
@@ -7099,7 +7113,7 @@
       <c r="B340" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C340" s="14" t="n">
+      <c r="C340" s="12" t="n">
         <v>43110</v>
       </c>
       <c r="D340" s="0" t="n">
@@ -7113,7 +7127,7 @@
       <c r="B341" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C341" s="14" t="n">
+      <c r="C341" s="12" t="n">
         <v>43110</v>
       </c>
       <c r="D341" s="13" t="n">
@@ -7127,7 +7141,7 @@
       <c r="B342" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C342" s="14" t="n">
+      <c r="C342" s="12" t="n">
         <v>43110</v>
       </c>
       <c r="D342" s="13" t="n">
@@ -7141,7 +7155,7 @@
       <c r="B343" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C343" s="14" t="n">
+      <c r="C343" s="12" t="n">
         <v>43110</v>
       </c>
       <c r="D343" s="13" t="n">
@@ -7155,7 +7169,7 @@
       <c r="B344" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C344" s="14" t="n">
+      <c r="C344" s="12" t="n">
         <v>43110</v>
       </c>
       <c r="D344" s="13" t="n">
@@ -7169,7 +7183,7 @@
       <c r="B345" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C345" s="14" t="n">
+      <c r="C345" s="12" t="n">
         <v>43110</v>
       </c>
       <c r="D345" s="13" t="n">
@@ -7183,7 +7197,7 @@
       <c r="B346" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C346" s="14" t="n">
+      <c r="C346" s="12" t="n">
         <v>43115</v>
       </c>
       <c r="D346" s="0" t="n">
@@ -7197,7 +7211,7 @@
       <c r="B347" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C347" s="14" t="n">
+      <c r="C347" s="12" t="n">
         <v>43115</v>
       </c>
       <c r="D347" s="13" t="n">
@@ -7211,7 +7225,7 @@
       <c r="B348" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C348" s="14" t="n">
+      <c r="C348" s="12" t="n">
         <v>43115</v>
       </c>
       <c r="D348" s="13" t="n">
@@ -7225,7 +7239,7 @@
       <c r="B349" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C349" s="14" t="n">
+      <c r="C349" s="12" t="n">
         <v>43115</v>
       </c>
       <c r="D349" s="13" t="n">
@@ -7239,7 +7253,7 @@
       <c r="B350" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C350" s="14" t="n">
+      <c r="C350" s="12" t="n">
         <v>43115</v>
       </c>
       <c r="D350" s="13" t="n">
@@ -7253,7 +7267,7 @@
       <c r="B351" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C351" s="14" t="n">
+      <c r="C351" s="12" t="n">
         <v>43115</v>
       </c>
       <c r="D351" s="13" t="n">
@@ -7267,7 +7281,7 @@
       <c r="B352" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C352" s="14" t="n">
+      <c r="C352" s="12" t="n">
         <v>43115</v>
       </c>
       <c r="D352" s="13" t="n">
@@ -7281,7 +7295,7 @@
       <c r="B353" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C353" s="14" t="n">
+      <c r="C353" s="12" t="n">
         <v>43115</v>
       </c>
       <c r="D353" s="13" t="n">
@@ -7295,7 +7309,7 @@
       <c r="B354" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C354" s="14" t="n">
+      <c r="C354" s="12" t="n">
         <v>43115</v>
       </c>
       <c r="D354" s="13" t="n">
@@ -7309,7 +7323,7 @@
       <c r="B355" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C355" s="14" t="n">
+      <c r="C355" s="12" t="n">
         <v>43115</v>
       </c>
       <c r="D355" s="13" t="n">
@@ -7323,7 +7337,7 @@
       <c r="B356" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C356" s="14" t="n">
+      <c r="C356" s="12" t="n">
         <v>43115</v>
       </c>
       <c r="D356" s="13" t="n">
@@ -7337,7 +7351,7 @@
       <c r="B357" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C357" s="14" t="n">
+      <c r="C357" s="12" t="n">
         <v>43119</v>
       </c>
       <c r="D357" s="0" t="n">
@@ -7351,7 +7365,7 @@
       <c r="B358" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C358" s="14" t="n">
+      <c r="C358" s="12" t="n">
         <v>43119</v>
       </c>
       <c r="D358" s="0" t="n">
@@ -7368,7 +7382,7 @@
       <c r="B359" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C359" s="14" t="n">
+      <c r="C359" s="12" t="n">
         <v>43119</v>
       </c>
       <c r="D359" s="0" t="n">
@@ -7382,7 +7396,7 @@
       <c r="B360" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C360" s="14" t="n">
+      <c r="C360" s="12" t="n">
         <v>43119</v>
       </c>
       <c r="D360" s="0" t="n">
@@ -7396,7 +7410,7 @@
       <c r="B361" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C361" s="14" t="n">
+      <c r="C361" s="12" t="n">
         <v>43119</v>
       </c>
       <c r="D361" s="0" t="n">
@@ -7410,7 +7424,7 @@
       <c r="B362" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C362" s="14" t="n">
+      <c r="C362" s="12" t="n">
         <v>43119</v>
       </c>
       <c r="D362" s="0" t="n">
@@ -7424,7 +7438,7 @@
       <c r="B363" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C363" s="14" t="n">
+      <c r="C363" s="12" t="n">
         <v>43129</v>
       </c>
       <c r="D363" s="13" t="n">
@@ -7438,7 +7452,7 @@
       <c r="B364" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C364" s="14" t="n">
+      <c r="C364" s="12" t="n">
         <v>43129</v>
       </c>
       <c r="D364" s="13" t="n">
@@ -7452,7 +7466,7 @@
       <c r="B365" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C365" s="14" t="n">
+      <c r="C365" s="12" t="n">
         <v>43129</v>
       </c>
       <c r="D365" s="13" t="n">
@@ -7466,7 +7480,7 @@
       <c r="B366" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C366" s="14" t="n">
+      <c r="C366" s="12" t="n">
         <v>43129</v>
       </c>
       <c r="D366" s="13" t="n">
@@ -7480,7 +7494,7 @@
       <c r="B367" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C367" s="14" t="n">
+      <c r="C367" s="12" t="n">
         <v>43129</v>
       </c>
       <c r="D367" s="13" t="n">
@@ -7494,7 +7508,7 @@
       <c r="B368" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C368" s="14" t="n">
+      <c r="C368" s="12" t="n">
         <v>43129</v>
       </c>
       <c r="D368" s="0" t="n">
@@ -7508,7 +7522,7 @@
       <c r="B369" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C369" s="14" t="n">
+      <c r="C369" s="12" t="n">
         <v>43129</v>
       </c>
       <c r="D369" s="0" t="n">
@@ -7525,7 +7539,7 @@
       <c r="B370" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C370" s="14" t="n">
+      <c r="C370" s="12" t="n">
         <v>43129</v>
       </c>
       <c r="D370" s="13" t="n">
@@ -7539,7 +7553,7 @@
       <c r="B371" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C371" s="14" t="n">
+      <c r="C371" s="12" t="n">
         <v>43129</v>
       </c>
       <c r="D371" s="13" t="n">
@@ -7553,7 +7567,7 @@
       <c r="B372" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C372" s="14" t="n">
+      <c r="C372" s="12" t="n">
         <v>43129</v>
       </c>
       <c r="D372" s="13" t="n">
@@ -7567,7 +7581,7 @@
       <c r="B373" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C373" s="14" t="n">
+      <c r="C373" s="12" t="n">
         <v>43129</v>
       </c>
       <c r="D373" s="13" t="n">
@@ -7581,7 +7595,7 @@
       <c r="B374" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C374" s="14" t="n">
+      <c r="C374" s="12" t="n">
         <v>43132</v>
       </c>
       <c r="D374" s="0" t="n">
@@ -7599,7 +7613,7 @@
       <c r="B375" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C375" s="14" t="n">
+      <c r="C375" s="12" t="n">
         <v>43132</v>
       </c>
       <c r="D375" s="13" t="n">
@@ -7620,7 +7634,7 @@
       <c r="B376" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C376" s="14" t="n">
+      <c r="C376" s="12" t="n">
         <v>43132</v>
       </c>
       <c r="D376" s="13" t="n">
@@ -7641,7 +7655,7 @@
       <c r="B377" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C377" s="14" t="n">
+      <c r="C377" s="12" t="n">
         <v>43132</v>
       </c>
       <c r="D377" s="13" t="n">
@@ -7659,7 +7673,7 @@
       <c r="B378" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C378" s="14" t="n">
+      <c r="C378" s="12" t="n">
         <v>43132</v>
       </c>
       <c r="D378" s="13" t="n">
@@ -7677,7 +7691,7 @@
       <c r="B379" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C379" s="14" t="n">
+      <c r="C379" s="12" t="n">
         <v>43132</v>
       </c>
       <c r="D379" s="13" t="n">
@@ -7695,7 +7709,7 @@
       <c r="B380" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C380" s="14" t="n">
+      <c r="C380" s="12" t="n">
         <v>43133</v>
       </c>
       <c r="D380" s="13" t="n">
@@ -7713,7 +7727,7 @@
       <c r="B381" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C381" s="14" t="n">
+      <c r="C381" s="12" t="n">
         <v>43133</v>
       </c>
       <c r="D381" s="13" t="n">
@@ -7734,7 +7748,7 @@
       <c r="B382" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C382" s="14" t="n">
+      <c r="C382" s="12" t="n">
         <v>43133</v>
       </c>
       <c r="D382" s="13" t="n">
@@ -7752,7 +7766,7 @@
       <c r="B383" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C383" s="14" t="n">
+      <c r="C383" s="12" t="n">
         <v>43133</v>
       </c>
       <c r="D383" s="13" t="n">
@@ -7770,7 +7784,7 @@
       <c r="B384" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C384" s="14" t="n">
+      <c r="C384" s="12" t="n">
         <v>43133</v>
       </c>
       <c r="D384" s="13" t="n">
@@ -7788,7 +7802,7 @@
       <c r="B385" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C385" s="14" t="n">
+      <c r="C385" s="12" t="n">
         <v>43137</v>
       </c>
       <c r="D385" s="0" t="n">
@@ -7802,7 +7816,7 @@
       <c r="B386" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C386" s="14" t="n">
+      <c r="C386" s="12" t="n">
         <v>43137</v>
       </c>
       <c r="D386" s="13" t="n">
@@ -7816,7 +7830,7 @@
       <c r="B387" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C387" s="14" t="n">
+      <c r="C387" s="12" t="n">
         <v>43137</v>
       </c>
       <c r="D387" s="13" t="n">
@@ -7830,7 +7844,7 @@
       <c r="B388" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C388" s="14" t="n">
+      <c r="C388" s="12" t="n">
         <v>43137</v>
       </c>
       <c r="D388" s="13" t="n">
@@ -7844,7 +7858,7 @@
       <c r="B389" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C389" s="14" t="n">
+      <c r="C389" s="12" t="n">
         <v>43137</v>
       </c>
       <c r="D389" s="13" t="n">
@@ -7858,7 +7872,7 @@
       <c r="B390" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C390" s="14" t="n">
+      <c r="C390" s="12" t="n">
         <v>43137</v>
       </c>
       <c r="D390" s="13" t="n">
@@ -7872,7 +7886,7 @@
       <c r="B391" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C391" s="14" t="n">
+      <c r="C391" s="12" t="n">
         <v>43137</v>
       </c>
       <c r="D391" s="13" t="n">
@@ -7886,7 +7900,7 @@
       <c r="B392" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C392" s="14" t="n">
+      <c r="C392" s="12" t="n">
         <v>43137</v>
       </c>
       <c r="D392" s="13" t="n">
@@ -7900,7 +7914,7 @@
       <c r="B393" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C393" s="14" t="n">
+      <c r="C393" s="12" t="n">
         <v>43137</v>
       </c>
       <c r="D393" s="13" t="n">
@@ -7914,7 +7928,7 @@
       <c r="B394" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C394" s="14" t="n">
+      <c r="C394" s="12" t="n">
         <v>43137</v>
       </c>
       <c r="D394" s="13" t="n">
@@ -7928,7 +7942,7 @@
       <c r="B395" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C395" s="14" t="n">
+      <c r="C395" s="12" t="n">
         <v>43137</v>
       </c>
       <c r="D395" s="13" t="n">
@@ -7942,7 +7956,7 @@
       <c r="B396" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C396" s="14" t="n">
+      <c r="C396" s="12" t="n">
         <v>43146</v>
       </c>
       <c r="D396" s="0" t="n">
@@ -7956,7 +7970,7 @@
       <c r="B397" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C397" s="14" t="n">
+      <c r="C397" s="12" t="n">
         <v>43146</v>
       </c>
       <c r="D397" s="13" t="n">
@@ -7970,7 +7984,7 @@
       <c r="B398" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C398" s="14" t="n">
+      <c r="C398" s="12" t="n">
         <v>43146</v>
       </c>
       <c r="D398" s="13" t="n">
@@ -7984,7 +7998,7 @@
       <c r="B399" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C399" s="14" t="n">
+      <c r="C399" s="12" t="n">
         <v>43146</v>
       </c>
       <c r="D399" s="13" t="n">
@@ -7998,7 +8012,7 @@
       <c r="B400" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C400" s="14" t="n">
+      <c r="C400" s="12" t="n">
         <v>43146</v>
       </c>
       <c r="D400" s="13" t="n">
@@ -8012,7 +8026,7 @@
       <c r="B401" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C401" s="14" t="n">
+      <c r="C401" s="12" t="n">
         <v>43146</v>
       </c>
       <c r="D401" s="13" t="n">
@@ -8026,7 +8040,7 @@
       <c r="B402" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C402" s="14" t="n">
+      <c r="C402" s="12" t="n">
         <v>43146</v>
       </c>
       <c r="D402" s="13" t="n">
@@ -8040,7 +8054,7 @@
       <c r="B403" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C403" s="14" t="n">
+      <c r="C403" s="12" t="n">
         <v>43146</v>
       </c>
       <c r="D403" s="13" t="n">
@@ -8054,7 +8068,7 @@
       <c r="B404" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C404" s="14" t="n">
+      <c r="C404" s="12" t="n">
         <v>43146</v>
       </c>
       <c r="D404" s="13" t="n">
@@ -8068,7 +8082,7 @@
       <c r="B405" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C405" s="14" t="n">
+      <c r="C405" s="12" t="n">
         <v>43146</v>
       </c>
       <c r="D405" s="13" t="n">
@@ -8082,7 +8096,7 @@
       <c r="B406" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C406" s="14" t="n">
+      <c r="C406" s="12" t="n">
         <v>43146</v>
       </c>
       <c r="D406" s="13" t="n">
@@ -8096,7 +8110,7 @@
       <c r="B407" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C407" s="14" t="n">
+      <c r="C407" s="12" t="n">
         <v>43147</v>
       </c>
       <c r="D407" s="0" t="n">
@@ -8110,7 +8124,7 @@
       <c r="B408" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C408" s="14" t="n">
+      <c r="C408" s="12" t="n">
         <v>43147</v>
       </c>
       <c r="D408" s="13" t="n">
@@ -8124,7 +8138,7 @@
       <c r="B409" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C409" s="14" t="n">
+      <c r="C409" s="12" t="n">
         <v>43147</v>
       </c>
       <c r="D409" s="13" t="n">
@@ -8138,7 +8152,7 @@
       <c r="B410" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C410" s="14" t="n">
+      <c r="C410" s="12" t="n">
         <v>43147</v>
       </c>
       <c r="D410" s="13" t="n">
@@ -8152,7 +8166,7 @@
       <c r="B411" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C411" s="14" t="n">
+      <c r="C411" s="12" t="n">
         <v>43147</v>
       </c>
       <c r="D411" s="13" t="n">
@@ -8166,7 +8180,7 @@
       <c r="B412" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C412" s="14" t="n">
+      <c r="C412" s="12" t="n">
         <v>43147</v>
       </c>
       <c r="D412" s="13" t="n">
@@ -8180,7 +8194,7 @@
       <c r="B413" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C413" s="14" t="n">
+      <c r="C413" s="12" t="n">
         <v>43153</v>
       </c>
       <c r="D413" s="0" t="n">
@@ -8194,7 +8208,7 @@
       <c r="B414" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C414" s="14" t="n">
+      <c r="C414" s="12" t="n">
         <v>43153</v>
       </c>
       <c r="D414" s="13" t="n">
@@ -8208,7 +8222,7 @@
       <c r="B415" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C415" s="14" t="n">
+      <c r="C415" s="12" t="n">
         <v>43153</v>
       </c>
       <c r="D415" s="13" t="n">
@@ -8222,7 +8236,7 @@
       <c r="B416" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C416" s="14" t="n">
+      <c r="C416" s="12" t="n">
         <v>43153</v>
       </c>
       <c r="D416" s="13" t="n">
@@ -8236,7 +8250,7 @@
       <c r="B417" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C417" s="14" t="n">
+      <c r="C417" s="12" t="n">
         <v>43153</v>
       </c>
       <c r="D417" s="13" t="n">
@@ -8250,7 +8264,7 @@
       <c r="B418" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C418" s="14" t="n">
+      <c r="C418" s="12" t="n">
         <v>43153</v>
       </c>
       <c r="D418" s="13" t="n">
@@ -8264,7 +8278,7 @@
       <c r="B419" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C419" s="14" t="n">
+      <c r="C419" s="12" t="n">
         <v>43153</v>
       </c>
       <c r="D419" s="13" t="n">
@@ -8278,7 +8292,7 @@
       <c r="B420" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C420" s="14" t="n">
+      <c r="C420" s="12" t="n">
         <v>43153</v>
       </c>
       <c r="D420" s="13" t="n">
@@ -8292,7 +8306,7 @@
       <c r="B421" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C421" s="14" t="n">
+      <c r="C421" s="12" t="n">
         <v>43153</v>
       </c>
       <c r="D421" s="13" t="n">
@@ -8306,7 +8320,7 @@
       <c r="B422" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C422" s="14" t="n">
+      <c r="C422" s="12" t="n">
         <v>43153</v>
       </c>
       <c r="D422" s="13" t="n">
@@ -8320,7 +8334,7 @@
       <c r="B423" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C423" s="14" t="n">
+      <c r="C423" s="12" t="n">
         <v>43153</v>
       </c>
       <c r="D423" s="13" t="n">
@@ -8334,7 +8348,7 @@
       <c r="B424" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C424" s="14" t="n">
+      <c r="C424" s="12" t="n">
         <v>43159</v>
       </c>
       <c r="D424" s="0" t="n">
@@ -8348,7 +8362,7 @@
       <c r="B425" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C425" s="14" t="n">
+      <c r="C425" s="12" t="n">
         <v>43159</v>
       </c>
       <c r="D425" s="13" t="n">
@@ -8362,7 +8376,7 @@
       <c r="B426" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C426" s="14" t="n">
+      <c r="C426" s="12" t="n">
         <v>43159</v>
       </c>
       <c r="D426" s="13" t="n">
@@ -8376,7 +8390,7 @@
       <c r="B427" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C427" s="14" t="n">
+      <c r="C427" s="12" t="n">
         <v>43159</v>
       </c>
       <c r="D427" s="13" t="n">
@@ -8390,7 +8404,7 @@
       <c r="B428" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C428" s="14" t="n">
+      <c r="C428" s="12" t="n">
         <v>43159</v>
       </c>
       <c r="D428" s="13" t="n">
@@ -8404,7 +8418,7 @@
       <c r="B429" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C429" s="14" t="n">
+      <c r="C429" s="12" t="n">
         <v>43159</v>
       </c>
       <c r="D429" s="13" t="n">
@@ -8418,7 +8432,7 @@
       <c r="B430" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C430" s="14" t="n">
+      <c r="C430" s="12" t="n">
         <v>43159</v>
       </c>
       <c r="D430" s="13" t="n">
@@ -8432,7 +8446,7 @@
       <c r="B431" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C431" s="14" t="n">
+      <c r="C431" s="12" t="n">
         <v>43159</v>
       </c>
       <c r="D431" s="13" t="n">
@@ -8446,7 +8460,7 @@
       <c r="B432" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C432" s="14" t="n">
+      <c r="C432" s="12" t="n">
         <v>43159</v>
       </c>
       <c r="D432" s="13" t="n">
@@ -8460,7 +8474,7 @@
       <c r="B433" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C433" s="14" t="n">
+      <c r="C433" s="12" t="n">
         <v>43159</v>
       </c>
       <c r="D433" s="13" t="n">
@@ -8474,7 +8488,7 @@
       <c r="B434" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C434" s="14" t="n">
+      <c r="C434" s="12" t="n">
         <v>43159</v>
       </c>
       <c r="D434" s="13" t="n">
@@ -8488,7 +8502,7 @@
       <c r="B435" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C435" s="14" t="n">
+      <c r="C435" s="12" t="n">
         <v>43167</v>
       </c>
       <c r="D435" s="13" t="n">
@@ -8502,7 +8516,7 @@
       <c r="B436" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C436" s="14" t="n">
+      <c r="C436" s="12" t="n">
         <v>43167</v>
       </c>
       <c r="D436" s="13" t="n">
@@ -8516,7 +8530,7 @@
       <c r="B437" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C437" s="14" t="n">
+      <c r="C437" s="12" t="n">
         <v>43167</v>
       </c>
       <c r="D437" s="13" t="n">
@@ -8530,7 +8544,7 @@
       <c r="B438" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C438" s="14" t="n">
+      <c r="C438" s="12" t="n">
         <v>43167</v>
       </c>
       <c r="D438" s="13" t="n">
@@ -8547,7 +8561,7 @@
       <c r="B439" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C439" s="14" t="n">
+      <c r="C439" s="12" t="n">
         <v>43167</v>
       </c>
       <c r="D439" s="13" t="n">
@@ -8561,7 +8575,7 @@
       <c r="B440" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C440" s="14" t="n">
+      <c r="C440" s="12" t="n">
         <v>43172</v>
       </c>
       <c r="D440" s="13" t="n">
@@ -8575,7 +8589,7 @@
       <c r="B441" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C441" s="14" t="n">
+      <c r="C441" s="12" t="n">
         <v>43172</v>
       </c>
       <c r="D441" s="13" t="n">
@@ -8589,7 +8603,7 @@
       <c r="B442" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C442" s="14" t="n">
+      <c r="C442" s="12" t="n">
         <v>43172</v>
       </c>
       <c r="D442" s="13" t="n">
@@ -8603,7 +8617,7 @@
       <c r="B443" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C443" s="14" t="n">
+      <c r="C443" s="12" t="n">
         <v>43172</v>
       </c>
       <c r="D443" s="13" t="n">
@@ -8617,7 +8631,7 @@
       <c r="B444" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C444" s="14" t="n">
+      <c r="C444" s="12" t="n">
         <v>43172</v>
       </c>
       <c r="D444" s="0" t="n">
@@ -8631,7 +8645,7 @@
       <c r="B445" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C445" s="14" t="n">
+      <c r="C445" s="12" t="n">
         <v>43172</v>
       </c>
       <c r="D445" s="13" t="n">
@@ -8645,7 +8659,7 @@
       <c r="B446" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C446" s="14" t="n">
+      <c r="C446" s="12" t="n">
         <v>43172</v>
       </c>
       <c r="D446" s="13" t="n">
@@ -8659,7 +8673,7 @@
       <c r="B447" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C447" s="14" t="n">
+      <c r="C447" s="12" t="n">
         <v>43172</v>
       </c>
       <c r="D447" s="13" t="n">
@@ -8673,7 +8687,7 @@
       <c r="B448" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C448" s="14" t="n">
+      <c r="C448" s="12" t="n">
         <v>43172</v>
       </c>
       <c r="D448" s="13" t="n">
@@ -8687,7 +8701,7 @@
       <c r="B449" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C449" s="14" t="n">
+      <c r="C449" s="12" t="n">
         <v>43172</v>
       </c>
       <c r="D449" s="13" t="n">
@@ -8701,7 +8715,7 @@
       <c r="B450" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C450" s="14" t="n">
+      <c r="C450" s="12" t="n">
         <v>43178</v>
       </c>
       <c r="D450" s="13" t="n">
@@ -8715,7 +8729,7 @@
       <c r="B451" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C451" s="14" t="n">
+      <c r="C451" s="12" t="n">
         <v>43178</v>
       </c>
       <c r="D451" s="13" t="n">
@@ -8732,7 +8746,7 @@
       <c r="B452" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C452" s="14" t="n">
+      <c r="C452" s="12" t="n">
         <v>43178</v>
       </c>
       <c r="D452" s="13" t="n">
@@ -8746,7 +8760,7 @@
       <c r="B453" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C453" s="14" t="n">
+      <c r="C453" s="12" t="n">
         <v>43178</v>
       </c>
       <c r="D453" s="13" t="n">
@@ -8756,7 +8770,1666 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="65536" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A454" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B454" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C454" s="12" t="n">
+        <v>43180</v>
+      </c>
+      <c r="D454" s="14" t="n">
+        <v>2215.2</v>
+      </c>
+      <c r="E454" s="14"/>
+      <c r="F454" s="14"/>
+    </row>
+    <row r="455" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A455" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B455" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C455" s="12" t="n">
+        <v>43180</v>
+      </c>
+      <c r="D455" s="15" t="n">
+        <v>8081.03</v>
+      </c>
+      <c r="E455" s="14"/>
+      <c r="F455" s="15" t="n">
+        <v>8081.03</v>
+      </c>
+    </row>
+    <row r="456" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A456" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B456" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C456" s="12" t="n">
+        <v>43180</v>
+      </c>
+      <c r="D456" s="15" t="n">
+        <v>43480.2</v>
+      </c>
+      <c r="E456" s="14"/>
+      <c r="F456" s="14"/>
+    </row>
+    <row r="457" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A457" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B457" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C457" s="12" t="n">
+        <v>43180</v>
+      </c>
+      <c r="D457" s="15" t="n">
+        <v>6343.67</v>
+      </c>
+      <c r="E457" s="14"/>
+      <c r="F457" s="14"/>
+    </row>
+    <row r="458" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A458" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B458" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C458" s="12" t="n">
+        <v>43180</v>
+      </c>
+      <c r="D458" s="15" t="n">
+        <v>12344.62</v>
+      </c>
+      <c r="E458" s="14"/>
+      <c r="F458" s="14"/>
+    </row>
+    <row r="459" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A459" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B459" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C459" s="12" t="n">
+        <v>43180</v>
+      </c>
+      <c r="D459" s="15" t="n">
+        <v>11119.69</v>
+      </c>
+      <c r="E459" s="14"/>
+      <c r="F459" s="14"/>
+    </row>
+    <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A460" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B460" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C460" s="12" t="n">
+        <v>43185</v>
+      </c>
+      <c r="D460" s="0" t="n">
+        <v>2208.96</v>
+      </c>
+    </row>
+    <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A461" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B461" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C461" s="12" t="n">
+        <v>43185</v>
+      </c>
+      <c r="D461" s="0" t="n">
+        <v>42520.1</v>
+      </c>
+    </row>
+    <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A462" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B462" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C462" s="12" t="n">
+        <v>43185</v>
+      </c>
+      <c r="D462" s="0" t="n">
+        <v>6349.5</v>
+      </c>
+    </row>
+    <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A463" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B463" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C463" s="12" t="n">
+        <v>43185</v>
+      </c>
+      <c r="D463" s="0" t="n">
+        <v>12589.79</v>
+      </c>
+      <c r="E463" s="0" t="n">
+        <v>11100</v>
+      </c>
+    </row>
+    <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A464" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B464" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C464" s="12" t="n">
+        <v>43185</v>
+      </c>
+      <c r="D464" s="0" t="n">
+        <v>11086.19</v>
+      </c>
+      <c r="F464" s="0" t="n">
+        <v>11086.19</v>
+      </c>
+    </row>
+    <row r="465" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A465" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B465" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C465" s="12" t="n">
+        <v>43185</v>
+      </c>
+      <c r="D465" s="13" t="n">
+        <v>14871.98</v>
+      </c>
+    </row>
+    <row r="466" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A466" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B466" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C466" s="12" t="n">
+        <v>43185</v>
+      </c>
+      <c r="D466" s="13" t="n">
+        <v>57532.57</v>
+      </c>
+    </row>
+    <row r="467" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A467" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B467" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C467" s="12" t="n">
+        <v>43185</v>
+      </c>
+      <c r="D467" s="13" t="n">
+        <v>12636.89</v>
+      </c>
+    </row>
+    <row r="468" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A468" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B468" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C468" s="12" t="n">
+        <v>43185</v>
+      </c>
+      <c r="D468" s="13" t="n">
+        <v>25972.11</v>
+      </c>
+    </row>
+    <row r="469" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A469" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B469" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C469" s="12" t="n">
+        <v>43186</v>
+      </c>
+      <c r="D469" s="13" t="n">
+        <v>14792.87</v>
+      </c>
+    </row>
+    <row r="470" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A470" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B470" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C470" s="12" t="n">
+        <v>43186</v>
+      </c>
+      <c r="D470" s="13" t="n">
+        <v>56704.28</v>
+      </c>
+      <c r="F470" s="0" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="471" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A471" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B471" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C471" s="12" t="n">
+        <v>43186</v>
+      </c>
+      <c r="D471" s="13" t="n">
+        <v>12640.52</v>
+      </c>
+    </row>
+    <row r="472" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A472" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B472" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C472" s="12" t="n">
+        <v>43186</v>
+      </c>
+      <c r="D472" s="13" t="n">
+        <v>25799.41</v>
+      </c>
+    </row>
+    <row r="473" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A473" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B473" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C473" s="12" t="n">
+        <v>43189</v>
+      </c>
+      <c r="D473" s="13" t="n">
+        <v>14790.08</v>
+      </c>
+    </row>
+    <row r="474" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A474" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B474" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C474" s="12" t="n">
+        <v>43189</v>
+      </c>
+      <c r="D474" s="13" t="n">
+        <v>55422.82</v>
+      </c>
+    </row>
+    <row r="475" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A475" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B475" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C475" s="12" t="n">
+        <v>43189</v>
+      </c>
+      <c r="D475" s="13" t="n">
+        <v>12651.43</v>
+      </c>
+    </row>
+    <row r="476" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A476" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B476" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C476" s="12" t="n">
+        <v>43189</v>
+      </c>
+      <c r="D476" s="13" t="n">
+        <v>25666.92</v>
+      </c>
+    </row>
+    <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A477" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B477" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C477" s="12" t="n">
+        <v>43189</v>
+      </c>
+      <c r="D477" s="0" t="n">
+        <v>2227.68</v>
+      </c>
+    </row>
+    <row r="478" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A478" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B478" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C478" s="12" t="n">
+        <v>43189</v>
+      </c>
+      <c r="D478" s="13" t="n">
+        <v>42089.86</v>
+      </c>
+    </row>
+    <row r="479" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A479" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B479" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C479" s="12" t="n">
+        <v>43189</v>
+      </c>
+      <c r="D479" s="13" t="n">
+        <v>6357.18</v>
+      </c>
+    </row>
+    <row r="480" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A480" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B480" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C480" s="12" t="n">
+        <v>43189</v>
+      </c>
+      <c r="D480" s="13" t="n">
+        <v>23540.7</v>
+      </c>
+    </row>
+    <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A481" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B481" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C481" s="12" t="n">
+        <v>43192</v>
+      </c>
+      <c r="D481" s="0" t="n">
+        <v>2241.2</v>
+      </c>
+    </row>
+    <row r="482" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A482" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B482" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C482" s="12" t="n">
+        <v>43192</v>
+      </c>
+      <c r="D482" s="13" t="n">
+        <v>42089.86</v>
+      </c>
+      <c r="H482" s="13"/>
+    </row>
+    <row r="483" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A483" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B483" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C483" s="12" t="n">
+        <v>43192</v>
+      </c>
+      <c r="D483" s="13" t="n">
+        <v>6357.18</v>
+      </c>
+      <c r="H483" s="13"/>
+    </row>
+    <row r="484" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A484" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B484" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C484" s="12" t="n">
+        <v>43192</v>
+      </c>
+      <c r="D484" s="13" t="n">
+        <v>23540.7</v>
+      </c>
+      <c r="E484" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H484" s="13"/>
+    </row>
+    <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A485" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B485" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C485" s="12" t="n">
+        <v>43192</v>
+      </c>
+      <c r="D485" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E485" s="0" t="n">
+        <v>2452.14</v>
+      </c>
+    </row>
+    <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A486" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B486" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C486" s="12" t="n">
+        <v>43193</v>
+      </c>
+      <c r="D486" s="0" t="n">
+        <v>2452.14</v>
+      </c>
+      <c r="E486" s="0" t="n">
+        <v>1981.07</v>
+      </c>
+    </row>
+    <row r="487" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A487" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B487" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C487" s="12" t="n">
+        <v>43193</v>
+      </c>
+      <c r="D487" s="13" t="n">
+        <v>14847.47</v>
+      </c>
+    </row>
+    <row r="488" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A488" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B488" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C488" s="12" t="n">
+        <v>43193</v>
+      </c>
+      <c r="D488" s="13" t="n">
+        <v>55981.37</v>
+      </c>
+      <c r="E488" s="13"/>
+      <c r="F488" s="0" t="n">
+        <v>15800</v>
+      </c>
+    </row>
+    <row r="489" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A489" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B489" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C489" s="12" t="n">
+        <v>43193</v>
+      </c>
+      <c r="D489" s="13" t="n">
+        <v>12655.07</v>
+      </c>
+      <c r="E489" s="13"/>
+    </row>
+    <row r="490" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A490" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B490" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C490" s="12" t="n">
+        <v>43193</v>
+      </c>
+      <c r="D490" s="13" t="n">
+        <v>26419.8</v>
+      </c>
+      <c r="E490" s="13"/>
+    </row>
+    <row r="491" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A491" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B491" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C491" s="12" t="n">
+        <v>43193</v>
+      </c>
+      <c r="D491" s="13" t="n">
+        <v>42489.65</v>
+      </c>
+      <c r="F491" s="0" t="n">
+        <v>6800</v>
+      </c>
+    </row>
+    <row r="492" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A492" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B492" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C492" s="12" t="n">
+        <v>43193</v>
+      </c>
+      <c r="D492" s="13" t="n">
+        <v>6359.1</v>
+      </c>
+    </row>
+    <row r="493" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A493" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B493" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C493" s="12" t="n">
+        <v>43193</v>
+      </c>
+      <c r="D493" s="13" t="n">
+        <f aca="false">23899.68+5000</f>
+        <v>28899.68</v>
+      </c>
+    </row>
+    <row r="494" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A494" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B494" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C494" s="12" t="n">
+        <v>43196</v>
+      </c>
+      <c r="D494" s="13" t="n">
+        <v>35843.43</v>
+      </c>
+    </row>
+    <row r="495" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A495" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B495" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C495" s="12" t="n">
+        <v>43196</v>
+      </c>
+      <c r="D495" s="13" t="n">
+        <v>6364.87</v>
+      </c>
+    </row>
+    <row r="496" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A496" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B496" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C496" s="12" t="n">
+        <v>43196</v>
+      </c>
+      <c r="D496" s="13" t="n">
+        <v>28681.44</v>
+      </c>
+      <c r="E496" s="0" t="n">
+        <v>6800</v>
+      </c>
+    </row>
+    <row r="497" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A497" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B497" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C497" s="12" t="n">
+        <v>43196</v>
+      </c>
+      <c r="D497" s="13" t="n">
+        <v>4428.45</v>
+      </c>
+    </row>
+    <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A498" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B498" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C498" s="12" t="n">
+        <v>43196</v>
+      </c>
+      <c r="D498" s="0" t="n">
+        <v>2238.08</v>
+      </c>
+    </row>
+    <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A499" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B499" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C499" s="12" t="n">
+        <v>43196</v>
+      </c>
+      <c r="D499" s="13" t="n">
+        <v>14845.64</v>
+      </c>
+    </row>
+    <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A500" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B500" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C500" s="12" t="n">
+        <v>43196</v>
+      </c>
+      <c r="D500" s="13" t="n">
+        <v>40449.67</v>
+      </c>
+    </row>
+    <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A501" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B501" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C501" s="12" t="n">
+        <v>43196</v>
+      </c>
+      <c r="D501" s="13" t="n">
+        <v>12665.99</v>
+      </c>
+    </row>
+    <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A502" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B502" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C502" s="12" t="n">
+        <v>43196</v>
+      </c>
+      <c r="D502" s="13" t="n">
+        <v>25826.54</v>
+      </c>
+      <c r="E502" s="0" t="n">
+        <v>14700</v>
+      </c>
+    </row>
+    <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A503" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B503" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C503" s="16" t="n">
+        <v>43200</v>
+      </c>
+      <c r="D503" s="13" t="n">
+        <v>14810.05</v>
+      </c>
+    </row>
+    <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A504" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B504" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C504" s="16" t="n">
+        <v>43200</v>
+      </c>
+      <c r="D504" s="13" t="n">
+        <v>39861.41</v>
+      </c>
+    </row>
+    <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A505" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B505" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C505" s="16" t="n">
+        <v>43200</v>
+      </c>
+      <c r="D505" s="13" t="n">
+        <v>12673.28</v>
+      </c>
+    </row>
+    <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A506" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B506" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C506" s="16" t="n">
+        <v>43200</v>
+      </c>
+      <c r="D506" s="0" t="n">
+        <f aca="false">26054.46 + 14700</f>
+        <v>40754.46</v>
+      </c>
+    </row>
+    <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A507" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B507" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C507" s="16" t="n">
+        <v>43200</v>
+      </c>
+      <c r="D507" s="13" t="n">
+        <v>35398.17</v>
+      </c>
+    </row>
+    <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A508" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B508" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C508" s="16" t="n">
+        <v>43200</v>
+      </c>
+      <c r="D508" s="13" t="n">
+        <v>6368.72</v>
+      </c>
+    </row>
+    <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A509" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B509" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C509" s="16" t="n">
+        <v>43200</v>
+      </c>
+      <c r="D509" s="0" t="n">
+        <f aca="false">28934.16+6800</f>
+        <v>35734.16</v>
+      </c>
+    </row>
+    <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A510" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B510" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C510" s="16" t="n">
+        <v>43200</v>
+      </c>
+      <c r="D510" s="13" t="n">
+        <v>4429.53</v>
+      </c>
+    </row>
+    <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A511" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B511" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C511" s="16" t="n">
+        <v>43202</v>
+      </c>
+      <c r="D511" s="13" t="n">
+        <v>36098.88</v>
+      </c>
+    </row>
+    <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A512" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B512" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C512" s="16" t="n">
+        <v>43202</v>
+      </c>
+      <c r="D512" s="13" t="n">
+        <v>6372.57</v>
+      </c>
+    </row>
+    <row r="513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A513" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B513" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C513" s="16" t="n">
+        <v>43202</v>
+      </c>
+      <c r="D513" s="13" t="n">
+        <v>35765.08</v>
+      </c>
+    </row>
+    <row r="514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A514" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B514" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C514" s="16" t="n">
+        <v>43202</v>
+      </c>
+      <c r="D514" s="13" t="n">
+        <v>4432.84</v>
+      </c>
+    </row>
+    <row r="515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A515" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B515" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C515" s="16" t="n">
+        <v>43202</v>
+      </c>
+      <c r="D515" s="13" t="n">
+        <v>14722.77</v>
+      </c>
+    </row>
+    <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A516" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B516" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C516" s="16" t="n">
+        <v>43202</v>
+      </c>
+      <c r="D516" s="13" t="n">
+        <v>40567.77</v>
+      </c>
+    </row>
+    <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A517" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B517" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C517" s="16" t="n">
+        <v>43202</v>
+      </c>
+      <c r="D517" s="13" t="n">
+        <v>12680.57</v>
+      </c>
+    </row>
+    <row r="518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A518" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B518" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C518" s="16" t="n">
+        <v>43202</v>
+      </c>
+      <c r="D518" s="13" t="n">
+        <v>40502.99</v>
+      </c>
+    </row>
+    <row r="519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A519" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B519" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C519" s="16" t="n">
+        <v>43202</v>
+      </c>
+      <c r="D519" s="0" t="n">
+        <f aca="false">2181.83+77.18+1.77</f>
+        <v>2260.78</v>
+      </c>
+      <c r="F519" s="0" t="n">
+        <f aca="false">2181.83+77.18+1.77</f>
+        <v>2260.78</v>
+      </c>
+    </row>
+    <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A520" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B520" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C520" s="16" t="n">
+        <v>43209</v>
+      </c>
+      <c r="D520" s="13" t="n">
+        <v>36526.85</v>
+      </c>
+    </row>
+    <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A521" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B521" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C521" s="16" t="n">
+        <v>43209</v>
+      </c>
+      <c r="D521" s="13" t="n">
+        <v>6382.21</v>
+      </c>
+    </row>
+    <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A522" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B522" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C522" s="16" t="n">
+        <v>43209</v>
+      </c>
+      <c r="D522" s="13" t="n">
+        <v>36081.85</v>
+      </c>
+    </row>
+    <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A523" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B523" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C523" s="16" t="n">
+        <v>43209</v>
+      </c>
+      <c r="D523" s="13" t="n">
+        <v>4438.34</v>
+      </c>
+    </row>
+    <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A524" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B524" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C524" s="16" t="n">
+        <v>43209</v>
+      </c>
+      <c r="D524" s="13" t="n">
+        <v>14600.27</v>
+      </c>
+    </row>
+    <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A525" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B525" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C525" s="16" t="n">
+        <v>43209</v>
+      </c>
+      <c r="D525" s="13" t="n">
+        <v>41230.66</v>
+      </c>
+    </row>
+    <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A526" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B526" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C526" s="16" t="n">
+        <v>43209</v>
+      </c>
+      <c r="D526" s="13" t="n">
+        <v>12698.82</v>
+      </c>
+    </row>
+    <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A527" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B527" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C527" s="16" t="n">
+        <v>43209</v>
+      </c>
+      <c r="D527" s="13" t="n">
+        <v>41218.12</v>
+      </c>
+    </row>
+    <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A528" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B528" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C528" s="16" t="n">
+        <v>43213</v>
+      </c>
+      <c r="D528" s="13" t="n">
+        <v>36382.89</v>
+      </c>
+    </row>
+    <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A529" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B529" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C529" s="16" t="n">
+        <v>43213</v>
+      </c>
+      <c r="D529" s="13" t="n">
+        <v>6386.07</v>
+      </c>
+    </row>
+    <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A530" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B530" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C530" s="16" t="n">
+        <v>43213</v>
+      </c>
+      <c r="D530" s="13" t="n">
+        <v>36508.29</v>
+      </c>
+    </row>
+    <row r="531" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A531" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B531" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C531" s="16" t="n">
+        <v>43213</v>
+      </c>
+      <c r="D531" s="13" t="n">
+        <v>4441.66</v>
+      </c>
+      <c r="F531" s="13" t="n">
+        <v>4441.66</v>
+      </c>
+    </row>
+    <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A532" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B532" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C532" s="16" t="n">
+        <v>43213</v>
+      </c>
+      <c r="D532" s="13" t="n">
+        <v>14805.91</v>
+      </c>
+    </row>
+    <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A533" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B533" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C533" s="16" t="n">
+        <v>43213</v>
+      </c>
+      <c r="D533" s="13" t="n">
+        <v>41066.16</v>
+      </c>
+    </row>
+    <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A534" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B534" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C534" s="16" t="n">
+        <v>43213</v>
+      </c>
+      <c r="D534" s="13" t="n">
+        <v>12706.12</v>
+      </c>
+    </row>
+    <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A535" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B535" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C535" s="16" t="n">
+        <v>43213</v>
+      </c>
+      <c r="D535" s="13" t="n">
+        <v>41704.81</v>
+      </c>
+    </row>
+    <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A536" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B536" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C536" s="16" t="n">
+        <v>43223</v>
+      </c>
+      <c r="D536" s="13" t="n">
+        <v>35908.81</v>
+      </c>
+    </row>
+    <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A537" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B537" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C537" s="16" t="n">
+        <v>43223</v>
+      </c>
+      <c r="D537" s="13" t="n">
+        <v>6399.6</v>
+      </c>
+    </row>
+    <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A538" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B538" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C538" s="16" t="n">
+        <v>43223</v>
+      </c>
+      <c r="D538" s="13" t="n">
+        <v>36746.2</v>
+      </c>
+    </row>
+    <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A539" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B539" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C539" s="16" t="n">
+        <v>43223</v>
+      </c>
+      <c r="D539" s="13" t="n">
+        <v>14684.72</v>
+      </c>
+      <c r="F539" s="13"/>
+    </row>
+    <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A540" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B540" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C540" s="16" t="n">
+        <v>43223</v>
+      </c>
+      <c r="D540" s="13" t="n">
+        <v>40524.41</v>
+      </c>
+    </row>
+    <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A541" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B541" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C541" s="16" t="n">
+        <v>43223</v>
+      </c>
+      <c r="D541" s="13" t="n">
+        <v>12731.73</v>
+      </c>
+    </row>
+    <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A542" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B542" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C542" s="16" t="n">
+        <v>43223</v>
+      </c>
+      <c r="D542" s="13" t="n">
+        <v>41976.36</v>
+      </c>
+    </row>
+    <row r="543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A543" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B543" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C543" s="16" t="n">
+        <v>43228</v>
+      </c>
+      <c r="D543" s="13" t="n">
+        <v>14052.97</v>
+      </c>
+    </row>
+    <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A544" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B544" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C544" s="16" t="n">
+        <v>43228</v>
+      </c>
+      <c r="D544" s="13" t="n">
+        <v>40759.45</v>
+      </c>
+    </row>
+    <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A545" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B545" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C545" s="16" t="n">
+        <v>43228</v>
+      </c>
+      <c r="D545" s="13" t="n">
+        <v>12742.72</v>
+      </c>
+    </row>
+    <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A546" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B546" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C546" s="16" t="n">
+        <v>43228</v>
+      </c>
+      <c r="D546" s="13" t="n">
+        <v>40643.1</v>
+      </c>
+    </row>
+    <row r="547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A547" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B547" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C547" s="16" t="n">
+        <v>43228</v>
+      </c>
+      <c r="D547" s="13" t="n">
+        <v>36120.34</v>
+      </c>
+    </row>
+    <row r="548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A548" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B548" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C548" s="16" t="n">
+        <v>43228</v>
+      </c>
+      <c r="D548" s="13" t="n">
+        <v>6405.41</v>
+      </c>
+    </row>
+    <row r="549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A549" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B549" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C549" s="16" t="n">
+        <v>43228</v>
+      </c>
+      <c r="D549" s="13" t="n">
+        <v>35578.07</v>
+      </c>
+    </row>
+    <row r="550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A550" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B550" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C550" s="16" t="n">
+        <v>43231</v>
+      </c>
+      <c r="D550" s="13" t="n">
+        <v>14332.51</v>
+      </c>
+    </row>
+    <row r="551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A551" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B551" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C551" s="16" t="n">
+        <v>43231</v>
+      </c>
+      <c r="D551" s="13" t="n">
+        <v>41474.83</v>
+      </c>
+    </row>
+    <row r="552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A552" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B552" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C552" s="16" t="n">
+        <v>43231</v>
+      </c>
+      <c r="D552" s="13" t="n">
+        <v>12753.71</v>
+      </c>
+    </row>
+    <row r="553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A553" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B553" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C553" s="16" t="n">
+        <v>43231</v>
+      </c>
+      <c r="D553" s="13" t="n">
+        <v>42092.09</v>
+      </c>
+    </row>
+    <row r="554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A554" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B554" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C554" s="16" t="n">
+        <v>43231</v>
+      </c>
+      <c r="D554" s="13" t="n">
+        <v>36758.82</v>
+      </c>
+    </row>
+    <row r="555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A555" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B555" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C555" s="16" t="n">
+        <v>43231</v>
+      </c>
+      <c r="D555" s="13" t="n">
+        <v>6411.22</v>
+      </c>
+    </row>
+    <row r="556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A556" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B556" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C556" s="16" t="n">
+        <v>43231</v>
+      </c>
+      <c r="D556" s="13" t="n">
+        <v>36847.6</v>
+      </c>
+    </row>
+    <row r="557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A557" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B557" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C557" s="16" t="n">
+        <v>43236</v>
+      </c>
+      <c r="D557" s="13" t="n">
+        <v>36274.78</v>
+      </c>
+    </row>
+    <row r="558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A558" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B558" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C558" s="16" t="n">
+        <v>43236</v>
+      </c>
+      <c r="D558" s="13" t="n">
+        <v>6417.04</v>
+      </c>
+    </row>
+    <row r="559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A559" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B559" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C559" s="16" t="n">
+        <v>43236</v>
+      </c>
+      <c r="D559" s="13" t="n">
+        <v>36660.86</v>
+      </c>
+      <c r="E559" s="0" t="n">
+        <v>2350</v>
+      </c>
+    </row>
+    <row r="560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A560" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B560" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C560" s="17" t="n">
+        <v>43255</v>
+      </c>
+      <c r="D560" s="13" t="n">
+        <v>13365.56</v>
+      </c>
+    </row>
+    <row r="561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A561" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B561" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C561" s="17" t="n">
+        <v>43255</v>
+      </c>
+      <c r="D561" s="13" t="n">
+        <v>41600.94</v>
+      </c>
+    </row>
+    <row r="562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A562" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B562" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C562" s="17" t="n">
+        <v>43255</v>
+      </c>
+      <c r="D562" s="13" t="n">
+        <v>12812.53</v>
+      </c>
+    </row>
+    <row r="563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A563" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B563" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C563" s="17" t="n">
+        <v>43255</v>
+      </c>
+      <c r="D563" s="13" t="n">
+        <v>37626.12</v>
+      </c>
+    </row>
+    <row r="564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A564" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B564" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C564" s="17" t="n">
+        <v>43255</v>
+      </c>
+      <c r="D564" s="13" t="n">
+        <v>36885.59</v>
+      </c>
+      <c r="E564" s="0" t="n">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A565" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B565" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C565" s="17" t="n">
+        <v>43255</v>
+      </c>
+      <c r="D565" s="13" t="n">
+        <v>6442.31</v>
+      </c>
+    </row>
+    <row r="566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A566" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B566" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C566" s="17" t="n">
+        <v>43255</v>
+      </c>
+      <c r="D566" s="13" t="n">
+        <v>35186.86</v>
+      </c>
+    </row>
+    <row r="65527" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>